<commit_message>
cleaned up network plots and added a narrative synthesis figure with the time series and international policy moments
</commit_message>
<xml_diff>
--- a/R/mitigation_factor_aesthetics2.xlsx
+++ b/R/mitigation_factor_aesthetics2.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="82">
   <si>
     <t>label</t>
   </si>
@@ -232,6 +232,39 @@
   </si>
   <si>
     <t>Opposition</t>
+  </si>
+  <si>
+    <t>label_varname</t>
+  </si>
+  <si>
+    <t>Publications (N)</t>
+  </si>
+  <si>
+    <t>Policy (N documents)</t>
+  </si>
+  <si>
+    <t>Legislation (N documents)</t>
+  </si>
+  <si>
+    <t>Interest (N posts)</t>
+  </si>
+  <si>
+    <t>Interest + Like (N posts + N likes)</t>
+  </si>
+  <si>
+    <t>Support (N posts)</t>
+  </si>
+  <si>
+    <t>Support agreement (N posts)</t>
+  </si>
+  <si>
+    <t>Support (Proportion of posts)</t>
+  </si>
+  <si>
+    <t>Opposition (N posts)</t>
+  </si>
+  <si>
+    <t>Action (various metrics)</t>
   </si>
 </sst>
 </file>
@@ -549,10 +582,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -562,7 +595,7 @@
     <col min="3" max="3" width="29.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -578,8 +611,11 @@
       <c r="E1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -596,7 +632,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -613,7 +649,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -630,7 +666,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -647,7 +683,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -664,7 +700,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -681,7 +717,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -698,7 +734,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -715,7 +751,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -732,7 +768,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -749,7 +785,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -766,7 +802,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -783,7 +819,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -800,7 +836,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -817,7 +853,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -834,7 +870,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>44</v>
       </c>
@@ -850,8 +886,11 @@
       <c r="E17" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -867,8 +906,11 @@
       <c r="E18" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F18" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>44</v>
       </c>
@@ -884,8 +926,11 @@
       <c r="E19" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>44</v>
       </c>
@@ -901,8 +946,11 @@
       <c r="E20" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>44</v>
       </c>
@@ -918,8 +966,11 @@
       <c r="E21" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F21" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>44</v>
       </c>
@@ -935,8 +986,11 @@
       <c r="E22" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -952,8 +1006,11 @@
       <c r="E23" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F23" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -969,8 +1026,11 @@
       <c r="E24" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F24" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>44</v>
       </c>
@@ -986,8 +1046,11 @@
       <c r="E25" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F25" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>44</v>
       </c>
@@ -1002,6 +1065,9 @@
       </c>
       <c r="E26" t="s">
         <v>64</v>
+      </c>
+      <c r="F26" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>